<commit_message>
feat: rename files as an example
</commit_message>
<xml_diff>
--- a/miniexcel/Students.xlsx
+++ b/miniexcel/Students.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="R3dd2bc443af444e6bb59ec358bfa8935"/>
+    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="Re20251412b5f40e8bd34f10efdfc2361"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -117,7 +117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:B12"/>
+  <x:dimension ref="A1:B13"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0">
       <x:pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -221,8 +221,16 @@
         <x:v>22</x:v>
       </x:c>
     </x:row>
+    <x:row r="13">
+      <x:c r="A13" t="str" s="2">
+        <x:v>sd</x:v>
+      </x:c>
+      <x:c r="B13" t="n" s="2">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:B12"/>
+  <x:autoFilter ref="A1:B13"/>
   <x:drawing r:id="drawing1"/>
 </x:worksheet>
 </file>
</xml_diff>